<commit_message>
Add distinction between identifier and abreviation for modules in the new import code
</commit_message>
<xml_diff>
--- a/FlOpEDT/configuration/file_essai.xlsx
+++ b/FlOpEDT/configuration/file_essai.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="5"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="4"/>
   </bookViews>
   <sheets>
     <sheet name="Paramètres" sheetId="1" state="visible" r:id="rId2"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="288" uniqueCount="175">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="300" uniqueCount="185">
   <si>
     <t xml:space="preserve">Dans cette feuille, trois sous-tableaux apparaissent.</t>
   </si>
@@ -429,6 +429,9 @@
     <t xml:space="preserve">Introduction à l’algorithmique</t>
   </si>
   <si>
+    <t xml:space="preserve">deux</t>
+  </si>
+  <si>
     <t xml:space="preserve">SDA</t>
   </si>
   <si>
@@ -438,6 +441,9 @@
     <t xml:space="preserve">Structures de données et algorithmes fondamentaux</t>
   </si>
   <si>
+    <t xml:space="preserve">trois</t>
+  </si>
+  <si>
     <t xml:space="preserve">IBD</t>
   </si>
   <si>
@@ -447,6 +453,9 @@
     <t xml:space="preserve">Introduction aux bases de données</t>
   </si>
   <si>
+    <t xml:space="preserve">quatre</t>
+  </si>
+  <si>
     <t xml:space="preserve">BDA</t>
   </si>
   <si>
@@ -456,6 +465,9 @@
     <t xml:space="preserve">Bases de données avancées</t>
   </si>
   <si>
+    <t xml:space="preserve">cinq</t>
+  </si>
+  <si>
     <t xml:space="preserve">PRST</t>
   </si>
   <si>
@@ -465,6 +477,9 @@
     <t xml:space="preserve">Probabilités et statistique</t>
   </si>
   <si>
+    <t xml:space="preserve">six</t>
+  </si>
+  <si>
     <t xml:space="preserve">MM</t>
   </si>
   <si>
@@ -474,6 +489,9 @@
     <t xml:space="preserve">Modélisations mathématiques</t>
   </si>
   <si>
+    <t xml:space="preserve">sept</t>
+  </si>
+  <si>
     <t xml:space="preserve">DTIC</t>
   </si>
   <si>
@@ -483,6 +501,9 @@
     <t xml:space="preserve">Droits des technologies de l’information et de la communication</t>
   </si>
   <si>
+    <t xml:space="preserve">huit</t>
+  </si>
+  <si>
     <t xml:space="preserve">GSI</t>
   </si>
   <si>
@@ -492,6 +513,9 @@
     <t xml:space="preserve">Gestion des systèmes d’information</t>
   </si>
   <si>
+    <t xml:space="preserve">neuf</t>
+  </si>
+  <si>
     <t xml:space="preserve">CP</t>
   </si>
   <si>
@@ -501,7 +525,7 @@
     <t xml:space="preserve">Communication professionnelle</t>
   </si>
   <si>
-    <t xml:space="preserve">CPAN</t>
+    <t xml:space="preserve">dix</t>
   </si>
   <si>
     <t xml:space="preserve">M3206</t>
@@ -510,7 +534,13 @@
     <t xml:space="preserve">Collaborer en anglais</t>
   </si>
   <si>
+    <t xml:space="preserve">pif</t>
+  </si>
+  <si>
     <t xml:space="preserve">Peu importe</t>
+  </si>
+  <si>
+    <t xml:space="preserve">paf</t>
   </si>
   <si>
     <t xml:space="preserve">Autre chose</t>
@@ -972,7 +1002,7 @@
       <selection pane="topLeft" activeCell="G8" activeCellId="0" sqref="G8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.55078125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.5703125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="24.6"/>
   </cols>
@@ -1224,7 +1254,7 @@
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="8" width="17.09"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="8" width="9.63"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="8" width="13.81"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="8" width="13.82"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="8" width="30.56"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="8" width="11.43"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="8" width="17.83"/>
@@ -1516,7 +1546,7 @@
   <dimension ref="A1:H33"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="G39" activeCellId="0" sqref="G39"/>
+      <selection pane="topLeft" activeCell="G38" activeCellId="0" sqref="G38"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -2440,21 +2470,21 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:I35"/>
+  <dimension ref="A1:J35"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="F21" activeCellId="0" sqref="F21"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="B19" activeCellId="0" sqref="B19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="8" width="18.8"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="8" width="17.21"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="8" width="52.58"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="8" width="17.52"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="8" width="15.28"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="8" width="20.6"/>
-    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1024" min="7" style="8" width="11.52"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="2" style="8" width="17.21"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="8" width="52.58"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="8" width="17.52"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="8" width="15.28"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="8" width="20.6"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1024" min="8" style="8" width="11.52"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2481,55 +2511,63 @@
       <c r="A5" s="23" t="s">
         <v>125</v>
       </c>
+      <c r="B5" s="23"/>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="23" t="s">
         <v>29</v>
       </c>
+      <c r="B6" s="23"/>
     </row>
     <row r="8" s="30" customFormat="true" ht="18.55" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="B8" s="2" t="s">
         <v>126</v>
       </c>
-      <c r="B8" s="2" t="s">
+      <c r="C8" s="2" t="s">
         <v>127</v>
       </c>
-      <c r="C8" s="2" t="s">
+      <c r="D8" s="2" t="s">
         <v>128</v>
       </c>
-      <c r="D8" s="2" t="s">
+      <c r="E8" s="2" t="s">
         <v>105</v>
       </c>
-      <c r="E8" s="2" t="s">
+      <c r="F8" s="2" t="s">
         <v>129</v>
       </c>
-      <c r="F8" s="2" t="s">
+      <c r="G8" s="2" t="s">
         <v>130</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A9" s="11" t="s">
+      <c r="A9" s="0" t="s">
+        <v>71</v>
+      </c>
+      <c r="B9" s="11" t="s">
         <v>131</v>
       </c>
-      <c r="B9" s="11" t="s">
+      <c r="C9" s="11" t="s">
         <v>132</v>
       </c>
-      <c r="C9" s="11" t="s">
+      <c r="D9" s="11" t="s">
         <v>133</v>
       </c>
-      <c r="D9" s="11" t="s">
+      <c r="E9" s="11" t="s">
         <v>88</v>
       </c>
-      <c r="E9" s="11" t="s">
+      <c r="F9" s="11" t="s">
         <v>24</v>
       </c>
-      <c r="F9" s="11" t="s">
+      <c r="G9" s="11" t="s">
         <v>36</v>
       </c>
-      <c r="I9" s="0"/>
+      <c r="J9" s="0"/>
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A10" s="11" t="s">
+      <c r="A10" s="0" t="s">
         <v>134</v>
       </c>
       <c r="B10" s="11" t="s">
@@ -2539,230 +2577,263 @@
         <v>136</v>
       </c>
       <c r="D10" s="11" t="s">
+        <v>137</v>
+      </c>
+      <c r="E10" s="11" t="s">
         <v>88</v>
       </c>
-      <c r="E10" s="11" t="s">
+      <c r="F10" s="11" t="s">
         <v>24</v>
       </c>
-      <c r="F10" s="11" t="s">
+      <c r="G10" s="11" t="s">
         <v>45</v>
       </c>
-      <c r="I10" s="0"/>
+      <c r="J10" s="0"/>
     </row>
     <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A11" s="11" t="s">
-        <v>137</v>
+      <c r="A11" s="0" t="s">
+        <v>138</v>
       </c>
       <c r="B11" s="11" t="s">
-        <v>138</v>
+        <v>139</v>
       </c>
       <c r="C11" s="11" t="s">
-        <v>139</v>
+        <v>140</v>
       </c>
       <c r="D11" s="11" t="s">
+        <v>141</v>
+      </c>
+      <c r="E11" s="11" t="s">
         <v>88</v>
       </c>
-      <c r="E11" s="11" t="s">
+      <c r="F11" s="11" t="s">
         <v>24</v>
       </c>
-      <c r="F11" s="11" t="s">
+      <c r="G11" s="11" t="s">
         <v>49</v>
       </c>
-      <c r="I11" s="0"/>
+      <c r="J11" s="0"/>
     </row>
     <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A12" s="11"/>
+      <c r="A12" s="0"/>
       <c r="B12" s="11"/>
       <c r="C12" s="11"/>
       <c r="D12" s="11"/>
       <c r="E12" s="11"/>
       <c r="F12" s="11"/>
-      <c r="I12" s="0"/>
+      <c r="G12" s="11"/>
+      <c r="J12" s="0"/>
     </row>
     <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A13" s="11" t="s">
-        <v>140</v>
+      <c r="A13" s="0" t="s">
+        <v>142</v>
       </c>
       <c r="B13" s="11" t="s">
-        <v>141</v>
+        <v>143</v>
       </c>
       <c r="C13" s="11" t="s">
-        <v>142</v>
+        <v>144</v>
       </c>
       <c r="D13" s="11" t="s">
+        <v>145</v>
+      </c>
+      <c r="E13" s="11" t="s">
         <v>90</v>
       </c>
-      <c r="E13" s="11" t="s">
+      <c r="F13" s="11" t="s">
         <v>26</v>
       </c>
-      <c r="F13" s="11" t="s">
+      <c r="G13" s="11" t="s">
         <v>45</v>
       </c>
-      <c r="I13" s="0"/>
+      <c r="J13" s="0"/>
     </row>
     <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A14" s="11" t="s">
-        <v>143</v>
+      <c r="A14" s="0" t="s">
+        <v>146</v>
       </c>
       <c r="B14" s="11" t="s">
-        <v>144</v>
+        <v>147</v>
       </c>
       <c r="C14" s="11" t="s">
-        <v>145</v>
+        <v>148</v>
       </c>
       <c r="D14" s="11" t="s">
+        <v>149</v>
+      </c>
+      <c r="E14" s="11" t="s">
         <v>90</v>
       </c>
-      <c r="E14" s="11" t="s">
+      <c r="F14" s="11" t="s">
         <v>26</v>
       </c>
-      <c r="F14" s="11" t="s">
+      <c r="G14" s="11" t="s">
         <v>36</v>
       </c>
-      <c r="I14" s="0"/>
+      <c r="J14" s="0"/>
     </row>
     <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A15" s="11" t="s">
-        <v>146</v>
+      <c r="A15" s="0" t="s">
+        <v>150</v>
       </c>
       <c r="B15" s="11" t="s">
-        <v>147</v>
+        <v>151</v>
       </c>
       <c r="C15" s="11" t="s">
-        <v>148</v>
+        <v>152</v>
       </c>
       <c r="D15" s="11" t="s">
+        <v>153</v>
+      </c>
+      <c r="E15" s="11" t="s">
         <v>90</v>
       </c>
-      <c r="E15" s="11" t="s">
+      <c r="F15" s="11" t="s">
         <v>26</v>
       </c>
-      <c r="F15" s="11" t="s">
+      <c r="G15" s="11" t="s">
         <v>49</v>
       </c>
-      <c r="I15" s="0"/>
+      <c r="J15" s="0"/>
     </row>
     <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A16" s="11" t="s">
-        <v>149</v>
+      <c r="A16" s="0" t="s">
+        <v>154</v>
       </c>
       <c r="B16" s="11" t="s">
-        <v>150</v>
+        <v>155</v>
       </c>
       <c r="C16" s="11" t="s">
-        <v>151</v>
+        <v>156</v>
       </c>
       <c r="D16" s="11" t="s">
+        <v>157</v>
+      </c>
+      <c r="E16" s="11" t="s">
         <v>90</v>
       </c>
-      <c r="E16" s="11" t="s">
+      <c r="F16" s="11" t="s">
         <v>26</v>
       </c>
-      <c r="F16" s="11" t="s">
+      <c r="G16" s="11" t="s">
         <v>45</v>
       </c>
-      <c r="I16" s="0"/>
+      <c r="J16" s="0"/>
     </row>
     <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A17" s="11" t="s">
-        <v>152</v>
+      <c r="A17" s="0" t="s">
+        <v>158</v>
       </c>
       <c r="B17" s="11" t="s">
-        <v>153</v>
+        <v>159</v>
       </c>
       <c r="C17" s="11" t="s">
-        <v>154</v>
+        <v>160</v>
       </c>
       <c r="D17" s="11" t="s">
+        <v>161</v>
+      </c>
+      <c r="E17" s="11" t="s">
         <v>90</v>
       </c>
-      <c r="E17" s="11" t="s">
+      <c r="F17" s="11" t="s">
         <v>26</v>
       </c>
-      <c r="F17" s="11" t="s">
+      <c r="G17" s="11" t="s">
         <v>49</v>
       </c>
-      <c r="I17" s="0"/>
+      <c r="J17" s="0"/>
     </row>
     <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A18" s="11" t="s">
-        <v>155</v>
+      <c r="A18" s="0" t="s">
+        <v>162</v>
       </c>
       <c r="B18" s="11" t="s">
-        <v>156</v>
+        <v>163</v>
       </c>
       <c r="C18" s="11" t="s">
-        <v>157</v>
+        <v>164</v>
       </c>
       <c r="D18" s="11" t="s">
+        <v>165</v>
+      </c>
+      <c r="E18" s="11" t="s">
         <v>90</v>
       </c>
-      <c r="E18" s="11" t="s">
+      <c r="F18" s="11" t="s">
         <v>26</v>
       </c>
-      <c r="F18" s="11" t="s">
+      <c r="G18" s="11" t="s">
         <v>45</v>
       </c>
-      <c r="I18" s="0"/>
+      <c r="J18" s="0"/>
     </row>
     <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A19" s="11" t="s">
-        <v>158</v>
-      </c>
-      <c r="B19" s="11" t="s">
-        <v>159</v>
-      </c>
+      <c r="A19" s="0" t="s">
+        <v>166</v>
+      </c>
+      <c r="B19" s="11"/>
       <c r="C19" s="11" t="s">
-        <v>160</v>
+        <v>167</v>
       </c>
       <c r="D19" s="11" t="s">
+        <v>168</v>
+      </c>
+      <c r="E19" s="11" t="s">
         <v>90</v>
       </c>
-      <c r="E19" s="11" t="s">
+      <c r="F19" s="11" t="s">
         <v>26</v>
       </c>
-      <c r="F19" s="11" t="s">
+      <c r="G19" s="11" t="s">
         <v>49</v>
       </c>
-      <c r="I19" s="0"/>
+      <c r="J19" s="0"/>
     </row>
     <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A20" s="11"/>
+      <c r="A20" s="0"/>
       <c r="B20" s="11"/>
       <c r="C20" s="11"/>
       <c r="D20" s="11"/>
       <c r="E20" s="11"/>
       <c r="F20" s="11"/>
+      <c r="G20" s="11"/>
     </row>
     <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A21" s="11" t="s">
+      <c r="A21" s="0" t="s">
         <v>73</v>
       </c>
-      <c r="B21" s="11"/>
-      <c r="C21" s="11" t="s">
-        <v>161</v>
-      </c>
+      <c r="B21" s="11" t="s">
+        <v>169</v>
+      </c>
+      <c r="C21" s="11"/>
       <c r="D21" s="11" t="s">
+        <v>170</v>
+      </c>
+      <c r="E21" s="11" t="s">
         <v>88</v>
       </c>
-      <c r="E21" s="11" t="s">
+      <c r="F21" s="11" t="s">
         <v>24</v>
       </c>
-      <c r="F21" s="11" t="s">
+      <c r="G21" s="11" t="s">
         <v>36</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A22" s="11" t="s">
+      <c r="A22" s="0" t="s">
         <v>73</v>
       </c>
-      <c r="B22" s="11"/>
-      <c r="C22" s="11" t="s">
-        <v>162</v>
-      </c>
-      <c r="D22" s="11"/>
+      <c r="B22" s="11" t="s">
+        <v>171</v>
+      </c>
+      <c r="C22" s="11"/>
+      <c r="D22" s="11" t="s">
+        <v>172</v>
+      </c>
       <c r="E22" s="11"/>
       <c r="F22" s="11"/>
+      <c r="G22" s="11"/>
     </row>
     <row r="23" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A23" s="11"/>
@@ -2771,6 +2842,7 @@
       <c r="D23" s="11"/>
       <c r="E23" s="11"/>
       <c r="F23" s="11"/>
+      <c r="G23" s="11"/>
     </row>
     <row r="24" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A24" s="11"/>
@@ -2779,6 +2851,7 @@
       <c r="D24" s="11"/>
       <c r="E24" s="11"/>
       <c r="F24" s="11"/>
+      <c r="G24" s="11"/>
     </row>
     <row r="25" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A25" s="11"/>
@@ -2787,6 +2860,7 @@
       <c r="D25" s="11"/>
       <c r="E25" s="11"/>
       <c r="F25" s="11"/>
+      <c r="G25" s="11"/>
     </row>
     <row r="26" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A26" s="11"/>
@@ -2795,6 +2869,7 @@
       <c r="D26" s="11"/>
       <c r="E26" s="11"/>
       <c r="F26" s="11"/>
+      <c r="G26" s="11"/>
     </row>
     <row r="27" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A27" s="11"/>
@@ -2803,6 +2878,7 @@
       <c r="D27" s="11"/>
       <c r="E27" s="11"/>
       <c r="F27" s="11"/>
+      <c r="G27" s="11"/>
     </row>
     <row r="28" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A28" s="11"/>
@@ -2811,6 +2887,7 @@
       <c r="D28" s="11"/>
       <c r="E28" s="11"/>
       <c r="F28" s="11"/>
+      <c r="G28" s="11"/>
     </row>
     <row r="29" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A29" s="11"/>
@@ -2819,6 +2896,7 @@
       <c r="D29" s="11"/>
       <c r="E29" s="11"/>
       <c r="F29" s="11"/>
+      <c r="G29" s="11"/>
     </row>
     <row r="30" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A30" s="11"/>
@@ -2827,6 +2905,7 @@
       <c r="D30" s="11"/>
       <c r="E30" s="11"/>
       <c r="F30" s="11"/>
+      <c r="G30" s="11"/>
     </row>
     <row r="31" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A31" s="11"/>
@@ -2835,6 +2914,7 @@
       <c r="D31" s="11"/>
       <c r="E31" s="11"/>
       <c r="F31" s="11"/>
+      <c r="G31" s="11"/>
     </row>
     <row r="32" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A32" s="11"/>
@@ -2843,6 +2923,7 @@
       <c r="D32" s="11"/>
       <c r="E32" s="11"/>
       <c r="F32" s="11"/>
+      <c r="G32" s="11"/>
     </row>
     <row r="33" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A33" s="11"/>
@@ -2851,6 +2932,7 @@
       <c r="D33" s="11"/>
       <c r="E33" s="11"/>
       <c r="F33" s="11"/>
+      <c r="G33" s="11"/>
     </row>
     <row r="34" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A34" s="11"/>
@@ -2859,6 +2941,7 @@
       <c r="D34" s="11"/>
       <c r="E34" s="11"/>
       <c r="F34" s="11"/>
+      <c r="G34" s="11"/>
     </row>
     <row r="35" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A35" s="11"/>
@@ -2867,18 +2950,19 @@
       <c r="D35" s="11"/>
       <c r="E35" s="11"/>
       <c r="F35" s="11"/>
+      <c r="G35" s="11"/>
     </row>
   </sheetData>
   <dataValidations count="3">
-    <dataValidation allowBlank="true" operator="equal" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="F9:F35" type="list">
+    <dataValidation allowBlank="true" operator="equal" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="G9:G35" type="list">
       <formula1>Intervenants!$A$6:$A$26</formula1>
       <formula2>0</formula2>
     </dataValidation>
-    <dataValidation allowBlank="true" operator="equal" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="E9:E35" type="list">
+    <dataValidation allowBlank="true" operator="equal" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="F9:F35" type="list">
       <formula1>Paramètres!$D$14:$D$23</formula1>
       <formula2>0</formula2>
     </dataValidation>
-    <dataValidation allowBlank="true" operator="equal" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="D9:D35" type="list">
+    <dataValidation allowBlank="true" operator="equal" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="E9:E35" type="list">
       <formula1>Groupes!$A$5:$A$11</formula1>
       <formula2>0</formula2>
     </dataValidation>
@@ -2900,8 +2984,8 @@
   </sheetPr>
   <dimension ref="A1:I22"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C16" activeCellId="0" sqref="C16"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="G14" activeCellId="0" sqref="G14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -2914,36 +2998,36 @@
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="31" t="s">
-        <v>163</v>
+        <v>173</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="31" t="s">
-        <v>164</v>
+        <v>174</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="31" t="s">
-        <v>165</v>
+        <v>175</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="31" t="s">
-        <v>166</v>
+        <v>176</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="31" t="s">
-        <v>167</v>
+        <v>177</v>
       </c>
       <c r="B5" s="8" t="n">
         <v>60</v>
       </c>
       <c r="C5" s="31" t="s">
-        <v>168</v>
+        <v>178</v>
       </c>
       <c r="D5" s="31" t="s">
-        <v>169</v>
+        <v>179</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2962,7 +3046,7 @@
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="32" t="s">
-        <v>170</v>
+        <v>180</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2972,13 +3056,13 @@
     </row>
     <row r="10" s="35" customFormat="true" ht="18.55" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="33" t="s">
-        <v>171</v>
+        <v>181</v>
       </c>
       <c r="B10" s="2" t="s">
-        <v>172</v>
+        <v>182</v>
       </c>
       <c r="C10" s="34" t="s">
-        <v>173</v>
+        <v>183</v>
       </c>
       <c r="D10" s="34"/>
       <c r="E10" s="34"/>
@@ -2989,7 +3073,7 @@
     </row>
     <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="36" t="s">
-        <v>167</v>
+        <v>177</v>
       </c>
       <c r="B11" s="29" t="n">
         <v>60</v>
@@ -3066,7 +3150,7 @@
     <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="36"/>
       <c r="B15" s="29" t="s">
-        <v>174</v>
+        <v>184</v>
       </c>
       <c r="C15" s="36"/>
       <c r="D15" s="36"/>

</xml_diff>